<commit_message>
Reviewed two scripts and updated Code_Structure.xlsx
</commit_message>
<xml_diff>
--- a/docs/Code_Structure.xlsx
+++ b/docs/Code_Structure.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_0D1F40DA42D4308E8830E1843AA8E7EF06BD8DC1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B73A358A-3AE3-411C-982F-93264AA1D264}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph.Lillington\PycharmProjects\NHP-flow-modelling\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A42EA-8B32-44C6-AE6F-A390273FC887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Folder</t>
   </si>
@@ -73,13 +78,43 @@
   </si>
   <si>
     <t>Scenario_tool.py</t>
+  </si>
+  <si>
+    <t>To read in parameters, primarily from config.json (but default parameters can be read from config_Edsizes.json and config_Edtypes.json if not supplied)</t>
+  </si>
+  <si>
+    <t>To provide model parameters</t>
+  </si>
+  <si>
+    <t>Functions are as follows:
+parse_config_acuity - Checks for errors on acuity percentages in config file
+parse_config_simtype - Checks if sim_parameters (daily number of patients, numbers of clinicans, maximum number of seats) has errors in config file
+parse_config_Sim_Parameters - Checks if several other sim_parameters have errors in config file
+get_EDtype_parameters - Return acuity percentages and various other sim parameters. 
+get_EDsize_parameters - Return ED size parameters
+get_target_time - Return target time, which affects time for decision to admit
+parse_bed_occupancy - Get bed time, which is time after decision to admit to actually get a bed.
+get_doctor_times - Get doctor times 
+get_diagnostic_percentages - Get diagnostic percentages
+-read_parameters - Read in input data using above functions.</t>
+  </si>
+  <si>
+    <t>Max_Waiting_Times - Max waiting time of patient before leaving  - i.e. their patience
+Prob_Admission - Is probability is admitted or dicharged</t>
+  </si>
+  <si>
+    <t>Do we want to have patient patience?
+Opening hours on rooms (SDEC has these).
+Numbers of doctors available doesn't depend on time of day
+Might want surge capacity beds because strict capacity constraints on certain rooms is likely unrealistic
+Many parameters are largely static (do not change depending on time of day) - need to think what we would want to model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,9 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,20 +494,20 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="61.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -499,8 +537,14 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -510,8 +554,17 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -522,7 +575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -539,6 +592,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6fbcc8e4-81ed-40b2-9b21-aa98bc8e658d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6303f13c-72cc-47f0-aeed-d46f93b29717">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003C3297AEF9452489C7FCE3B7D0A0240" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1bacd8e428934135053ba814caf68e07">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6303f13c-72cc-47f0-aeed-d46f93b29717" xmlns:ns3="6fbcc8e4-81ed-40b2-9b21-aa98bc8e658d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="61018ef9cd4e089a50c2ac4547d3a346" ns2:_="" ns3:_="">
     <xsd:import namespace="6303f13c-72cc-47f0-aeed-d46f93b29717"/>
@@ -787,34 +860,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6fbcc8e4-81ed-40b2-9b21-aa98bc8e658d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6303f13c-72cc-47f0-aeed-d46f93b29717">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3221171-99EA-4B89-8ABF-936A32F977DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B872B4-34D4-4644-A22A-DC2C35E291A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B872B4-34D4-4644-A22A-DC2C35E291A7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A22D81-4F1F-4B11-9342-4D7DA029D33D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6fbcc8e4-81ed-40b2-9b21-aa98bc8e658d"/>
+    <ds:schemaRef ds:uri="6303f13c-72cc-47f0-aeed-d46f93b29717"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A22D81-4F1F-4B11-9342-4D7DA029D33D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3221171-99EA-4B89-8ABF-936A32F977DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6303f13c-72cc-47f0-aeed-d46f93b29717"/>
+    <ds:schemaRef ds:uri="6fbcc8e4-81ed-40b2-9b21-aa98bc8e658d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reviewed Process_mapping.R and Analyse_MC_Tool_data.py
</commit_message>
<xml_diff>
--- a/docs/Code_Structure.xlsx
+++ b/docs/Code_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph.Lillington\PycharmProjects\NHP-flow-modelling\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3542E402-FA66-4F70-B82F-33C6A18B9CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA672BC-0748-4E83-97A1-7BD157EE861E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>Folder</t>
   </si>
@@ -213,6 +213,27 @@
   </si>
   <si>
     <t>Joe- Suggest Ignore</t>
+  </si>
+  <si>
+    <t>Script for performing process mining on model output data. This is useful for validating modelling pathway and for understanding bottlenecks in model</t>
+  </si>
+  <si>
+    <t>There's a whole host of graphs produced in this script, both for process maps and for general EA. 
+Think it would be worth using this as the basis for all outputs and going away from other png files, below.</t>
+  </si>
+  <si>
+    <t>Reads in distribution_outputs.csv  data from deterministic simulations, only.
+Is run after running model 
+Reads event log data</t>
+  </si>
+  <si>
+    <t>Analyse Monte-Carlo data</t>
+  </si>
+  <si>
+    <t>Reads in monte_carlo_table.csv (simple data on discharge time and admission time) and computes  statistics across runs looking at variability of 4 hr percentages.</t>
+  </si>
+  <si>
+    <t>Might want to expand script to not only look at 4 hr percentages, but a range of other metrics. Suggest adjusting monte_carlo_table to take full event logs, as in distribution_outputs.csv not only discharge and admission times.</t>
   </si>
 </sst>
 </file>
@@ -598,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,7 +809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -799,7 +820,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -810,7 +831,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -821,7 +842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -832,7 +853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -842,8 +863,17 @@
       <c r="C21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -853,8 +883,17 @@
       <c r="C22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -862,7 +901,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -876,15 +915,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003C3297AEF9452489C7FCE3B7D0A0240" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1bacd8e428934135053ba814caf68e07">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6303f13c-72cc-47f0-aeed-d46f93b29717" xmlns:ns3="6fbcc8e4-81ed-40b2-9b21-aa98bc8e658d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="61018ef9cd4e089a50c2ac4547d3a346" ns2:_="" ns3:_="">
     <xsd:import namespace="6303f13c-72cc-47f0-aeed-d46f93b29717"/>
@@ -1133,6 +1163,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1145,14 +1184,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B872B4-34D4-4644-A22A-DC2C35E291A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3221171-99EA-4B89-8ABF-936A32F977DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1171,6 +1202,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B872B4-34D4-4644-A22A-DC2C35E291A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A22D81-4F1F-4B11-9342-4D7DA029D33D}">
   <ds:schemaRefs>

</xml_diff>